<commit_message>
adding Šalamúnová Mária to Klobucka kola
</commit_message>
<xml_diff>
--- a/2024/02-klobuckaKola/02-VKCT2024-KlobuckaKola.xlsx
+++ b/2024/02-klobuckaKola/02-VKCT2024-KlobuckaKola.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Předškoláci I" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="242">
   <si>
     <t xml:space="preserve">KATEGORIE</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t xml:space="preserve">00:32:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Šalamúnová Mária</t>
   </si>
   <si>
     <t xml:space="preserve">Mladší žáci (2012-2013)</t>
@@ -1614,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -1654,7 +1657,7 @@
         <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2010</v>
@@ -1663,7 +1666,7 @@
         <v>81</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -1676,7 +1679,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2010</v>
@@ -1685,7 +1688,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2</v>
@@ -1698,16 +1701,16 @@
         <v>77</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2011</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>3</v>
@@ -1720,7 +1723,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2010</v>
@@ -1729,7 +1732,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>4</v>
@@ -2107,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -2152,16 +2155,16 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2007</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -2569,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -2614,16 +2617,16 @@
         <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2009</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -3031,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -3481,7 +3484,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -3526,16 +3529,16 @@
         <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1972</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -3548,16 +3551,16 @@
         <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1974</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2</v>
@@ -3955,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -4000,16 +4003,16 @@
         <v>104</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2005</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -4022,16 +4025,16 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1992</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2</v>
@@ -4044,16 +4047,16 @@
         <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1992</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>3</v>
@@ -4066,7 +4069,7 @@
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2006</v>
@@ -4075,7 +4078,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>4</v>
@@ -4088,16 +4091,16 @@
         <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1986</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>5</v>
@@ -4444,7 +4447,7 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4465,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -4510,16 +4513,16 @@
         <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1977</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -4532,16 +4535,16 @@
         <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1975</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2</v>
@@ -4554,16 +4557,16 @@
         <v>111</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1976</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>3</v>
@@ -4576,16 +4579,16 @@
         <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1977</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>4</v>
@@ -4963,7 +4966,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -5008,14 +5011,14 @@
         <v>108</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1971</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -5028,16 +5031,16 @@
         <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1972</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2</v>
@@ -5050,7 +5053,7 @@
         <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1971</v>
@@ -5059,7 +5062,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>3</v>
@@ -5072,14 +5075,14 @@
         <v>114</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1974</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>4</v>
@@ -5092,16 +5095,16 @@
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1972</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>5</v>
@@ -5114,16 +5117,16 @@
         <v>120</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>1972</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>6</v>
@@ -8795,8 +8798,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8897,11 +8900,17 @@
     </row>
     <row r="6" s="8" customFormat="true" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2011</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10" t="n">
+        <v>3</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="9"/>
     </row>
@@ -9285,7 +9294,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -9325,7 +9334,7 @@
         <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2012</v>
@@ -9334,7 +9343,7 @@
         <v>81</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -9347,16 +9356,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2013</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2</v>
@@ -9378,7 +9387,7 @@
         <v>107</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>3</v>
@@ -9391,16 +9400,16 @@
         <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2013</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>4</v>
@@ -9413,16 +9422,16 @@
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>2013</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>5</v>
@@ -9435,13 +9444,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>2013</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>137</v>
@@ -9457,7 +9466,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>2012</v>
@@ -9466,7 +9475,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>7</v>
@@ -9479,7 +9488,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>2013</v>
@@ -9488,7 +9497,7 @@
         <v>39</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>8</v>

</xml_diff>